<commit_message>
docs: add radio control wiring details for corvon_V5
</commit_message>
<xml_diff>
--- a/docs/assets/flight_controller/corvon_V5/corvon_V5_pinout.xlsx
+++ b/docs/assets/flight_controller/corvon_V5/corvon_V5_pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21940"/>
+    <workbookView windowWidth="27880" windowHeight="14400"/>
   </bookViews>
   <sheets>
     <sheet name="All Pinouts" sheetId="2" r:id="rId1"/>
@@ -27,44 +27,16 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="E118" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="SimSun"/>
-            <charset val="134"/>
-          </rPr>
-          <t>Used to Set MUX for Serial ESC or CAN Silent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E121" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="SimSun"/>
-            <charset val="134"/>
-          </rPr>
-          <t>Added 11/22 - to support EEPROM</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="514">
   <si>
     <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">corvon_V5 pinouts </t>
     </r>
     <r>
@@ -1628,7 +1600,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1832,11 +1804,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="SimSun"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -3132,9 +3099,9 @@
   <dimension ref="A1:L1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.2890625" defaultRowHeight="15" customHeight="1"/>
@@ -13086,7 +13053,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
   <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>